<commit_message>
Add function to push persents into time_stat.xlsc.
</commit_message>
<xml_diff>
--- a/time_stat.xlsx
+++ b/time_stat.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:G2"/>
@@ -534,13 +534,198 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>83</v>
+        <v>300</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>225</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="3" t="n">
+        <v>1.111111111111111</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="3" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="3" t="n">
+        <v>2.222222222222222</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" s="3" t="n">
+        <v>2.777777777777778</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="3" t="n">
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" s="3" t="n">
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" s="3" t="n">
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" s="3" t="n">
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>